<commit_message>
Updated plots a bit.
</commit_message>
<xml_diff>
--- a/docs/NormalsSharedMem.xlsx
+++ b/docs/NormalsSharedMem.xlsx
@@ -105,10 +105,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Sheet1!$A$3:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -123,19 +123,16 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:f>Sheet1!$B$3:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>63</c:v>
                 </c:pt>
@@ -150,9 +147,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -174,10 +168,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Sheet1!$A$3:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -192,19 +186,16 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$8</c:f>
+              <c:f>Sheet1!$C$3:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>53</c:v>
                 </c:pt>
@@ -219,9 +210,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -333,10 +321,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Sheet1!$A$3:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -351,19 +339,16 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$8</c:f>
+              <c:f>Sheet1!$D$3:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>5.5</c:v>
                 </c:pt>
@@ -378,9 +363,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -402,10 +384,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Sheet1!$A$3:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -420,19 +402,16 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$8</c:f>
+              <c:f>Sheet1!$E$3:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>8.5</c:v>
                 </c:pt>
@@ -447,9 +426,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>119.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>457</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -571,15 +547,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -888,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>